<commit_message>
Commit a porra toda
</commit_message>
<xml_diff>
--- a/Project1/attibutesStats.xlsx
+++ b/Project1/attibutesStats.xlsx
@@ -398,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -417,8 +417,20 @@
       <c r="D1" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -426,13 +438,25 @@
         <v>138.3268398268398</v>
       </c>
       <c r="C2">
-        <v>20.47412299767998</v>
+        <v>20.49631717546763</v>
       </c>
       <c r="D2">
-        <v>419.1897125241281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>420.0990177573692</v>
+      </c>
+      <c r="E2">
+        <v>134</v>
+      </c>
+      <c r="F2">
+        <v>218</v>
+      </c>
+      <c r="G2">
+        <v>101</v>
+      </c>
+      <c r="H2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -440,13 +464,25 @@
         <v>3.635649350649351</v>
       </c>
       <c r="C3">
-        <v>4.588050580380221</v>
+        <v>4.593024078404592</v>
       </c>
       <c r="D3">
-        <v>21.05020812812728</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>21.09587018480435</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>31.2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -454,13 +490,25 @@
         <v>4.740324675324675</v>
       </c>
       <c r="C4">
-        <v>2.068666703269999</v>
+        <v>2.070909161059325</v>
       </c>
       <c r="D4">
-        <v>4.279381929217968</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>4.288664753359439</v>
+      </c>
+      <c r="E4">
+        <v>4.34</v>
+      </c>
+      <c r="F4">
+        <v>15.33</v>
+      </c>
+      <c r="G4">
+        <v>0.98</v>
+      </c>
+      <c r="H4">
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -468,13 +516,25 @@
         <v>25.4067316017316</v>
       </c>
       <c r="C5">
-        <v>7.77227336478631</v>
+        <v>7.780698595839763</v>
       </c>
       <c r="D5">
-        <v>60.4082332569667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>60.53927063930286</v>
+      </c>
+      <c r="E5">
+        <v>26.115</v>
+      </c>
+      <c r="F5">
+        <v>42.49</v>
+      </c>
+      <c r="G5">
+        <v>6.74</v>
+      </c>
+      <c r="H5">
+        <v>35.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -482,13 +542,25 @@
         <v>0.4155844155844156</v>
       </c>
       <c r="C6">
-        <v>0.4928224924937734</v>
+        <v>0.4933567175747401</v>
       </c>
       <c r="D6">
-        <v>0.2428740091077753</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.2434008507761219</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -496,13 +568,25 @@
         <v>53.1038961038961</v>
       </c>
       <c r="C7">
-        <v>9.806903322952786</v>
+        <v>9.817534115584078</v>
       </c>
       <c r="D7">
-        <v>96.17535278574239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>96.38397611065723</v>
+      </c>
+      <c r="E7">
+        <v>53</v>
+      </c>
+      <c r="F7">
+        <v>78</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -510,13 +594,25 @@
         <v>26.04411255411255</v>
       </c>
       <c r="C8">
-        <v>4.209117496564533</v>
+        <v>4.213680226897766</v>
       </c>
       <c r="D8">
-        <v>17.71667009988568</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>17.75510105454921</v>
+      </c>
+      <c r="E8">
+        <v>25.805</v>
+      </c>
+      <c r="F8">
+        <v>46.58</v>
+      </c>
+      <c r="G8">
+        <v>14.7</v>
+      </c>
+      <c r="H8">
+        <v>31.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -524,13 +620,25 @@
         <v>17.04439393939393</v>
       </c>
       <c r="C9">
-        <v>24.45454968692465</v>
+        <v>24.48105869165857</v>
       </c>
       <c r="D9">
-        <v>598.0250003902663</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>599.3222346644318</v>
+      </c>
+      <c r="E9">
+        <v>7.51</v>
+      </c>
+      <c r="F9">
+        <v>147.19</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>147.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -538,10 +646,22 @@
         <v>42.81601731601732</v>
       </c>
       <c r="C10">
-        <v>14.59313732086082</v>
+        <v>14.60895644455249</v>
       </c>
       <c r="D10">
-        <v>212.959656865501</v>
+        <v>213.4216083988318</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>64</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>